<commit_message>
Removed redundant calls when creating update callbacks.
</commit_message>
<xml_diff>
--- a/ExcelTools/Test_Files/manual data load test.xlsx
+++ b/ExcelTools/Test_Files/manual data load test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18372" windowHeight="6852" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18375" windowHeight="6855" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Substance Creation" sheetId="1" r:id="rId1"/>
@@ -165,7 +165,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="55">
   <si>
     <t>BATCH:Create Substance</t>
   </si>
@@ -290,19 +290,46 @@
     <t>New Sub1</t>
   </si>
   <si>
-    <t>Real simple test</t>
-  </si>
-  <si>
     <t>cn</t>
   </si>
   <si>
     <t>blah</t>
   </si>
   <si>
-    <t>blah: blah2; blah3</t>
-  </si>
-  <si>
     <t>JOURNAL ARTICLE</t>
+  </si>
+  <si>
+    <t>Another synonym</t>
+  </si>
+  <si>
+    <t>blah again</t>
+  </si>
+  <si>
+    <t>Adding another name</t>
+  </si>
+  <si>
+    <t>5259a1b9-1627-4431-8fce-5bceb15ce47c</t>
+  </si>
+  <si>
+    <t>a5fe114a-d4e9-4f13-bc75-1503423a7a7d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nicotine </t>
+  </si>
+  <si>
+    <t>(-)-3-(1-Methyl-2-pyrrolidyl)pyridine</t>
+  </si>
+  <si>
+    <t>nicotine</t>
+  </si>
+  <si>
+    <t>https://chem.nlm.nih.gov/chemidplus/name/nicotine</t>
+  </si>
+  <si>
+    <t>adding a name</t>
+  </si>
+  <si>
+    <t>SYS</t>
   </si>
 </sst>
 </file>
@@ -1172,28 +1199,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.44140625" customWidth="1"/>
+    <col min="1" max="1" width="27.42578125" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.109375" customWidth="1"/>
-    <col min="7" max="7" width="8.44140625" customWidth="1"/>
-    <col min="8" max="8" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.140625" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3.44140625" customWidth="1"/>
-    <col min="13" max="13" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.42578125" customWidth="1"/>
+    <col min="13" max="13" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1234,7 +1261,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>22</v>
@@ -1269,7 +1296,7 @@
       </c>
       <c r="M2" s="3"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>24</v>
       </c>
@@ -1314,29 +1341,29 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.140625" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="10.44140625" customWidth="1"/>
-    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>34</v>
       </c>
@@ -1374,7 +1401,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>33</v>
       </c>
@@ -1402,11 +1429,8 @@
       <c r="J2" t="s">
         <v>38</v>
       </c>
-      <c r="K2" t="s">
-        <v>28</v>
-      </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>39</v>
       </c>
@@ -1414,25 +1438,83 @@
         <v>40</v>
       </c>
       <c r="D4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" t="s">
         <v>41</v>
-      </c>
-      <c r="E4" t="s">
-        <v>42</v>
       </c>
       <c r="F4" t="s">
         <v>21</v>
       </c>
       <c r="G4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4" t="s">
+        <v>42</v>
+      </c>
+      <c r="I4" t="s">
         <v>45</v>
       </c>
-      <c r="H4" t="s">
-        <v>43</v>
-      </c>
-      <c r="I4" t="s">
-        <v>44</v>
-      </c>
       <c r="J4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>